<commit_message>
updated variables and data for charts
</commit_message>
<xml_diff>
--- a/generator/data/generated_business_labels_map.xlsx
+++ b/generator/data/generated_business_labels_map.xlsx
@@ -6161,7 +6161,7 @@
         <v>112</v>
       </c>
       <c r="J72">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K72" t="s">
         <v>774</v>
@@ -6231,7 +6231,7 @@
         <v>112</v>
       </c>
       <c r="J74">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K74" t="s">
         <v>776</v>
@@ -6919,7 +6919,7 @@
         <v>112</v>
       </c>
       <c r="J94">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K94" t="s">
         <v>796</v>
@@ -7129,7 +7129,7 @@
         <v>112</v>
       </c>
       <c r="J100">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K100" t="s">
         <v>802</v>

</xml_diff>